<commit_message>
Segerated EnvFIiles and Added feature columns
</commit_message>
<xml_diff>
--- a/EnvNP_Cambodia.xlsx
+++ b/EnvNP_Cambodia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuvvvvv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B510B93-1336-3948-8CE0-8F6D0F430121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF27A61-2124-6746-B6F0-CE32A0971C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15320" xr2:uid="{1A7D7434-B2D3-7644-850A-F97E7EFCB430}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
   <si>
     <t>Mlup Baitong</t>
   </si>
@@ -204,6 +204,36 @@
 - INSTITUTIONAL &amp; COMMUNITY CAPACITING
 - AGRICULTURAL &amp; WATER RESOURCE MANAGEMENT
 - ENGAGEMENT PROGRAMS</t>
+  </si>
+  <si>
+    <t>Name of organisation</t>
+  </si>
+  <si>
+    <t>Description of organisation</t>
+  </si>
+  <si>
+    <t>Mission/ Objectives/ Purpose</t>
+  </si>
+  <si>
+    <t>Programmes/ projects</t>
+  </si>
+  <si>
+    <t>Funding sources</t>
+  </si>
+  <si>
+    <t>Collaboration with government / businesses</t>
+  </si>
+  <si>
+    <t>Choice of Climate action</t>
+  </si>
+  <si>
+    <t>No. of employees</t>
+  </si>
+  <si>
+    <t>Geographical focus</t>
+  </si>
+  <si>
+    <t>Nationality</t>
   </si>
 </sst>
 </file>
@@ -232,12 +262,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -252,12 +288,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -574,70 +613,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912F30BA-C468-F340-95C6-D349650C08A4}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J8"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
+    <row r="1" spans="1:10" ht="57" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2">
         <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>8</v>
@@ -646,30 +685,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2">
         <v>6</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>8</v>
@@ -680,28 +719,28 @@
     </row>
     <row r="4" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="2">
-        <v>1</v>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>8</v>
@@ -712,19 +751,19 @@
     </row>
     <row r="5" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>14</v>
@@ -733,7 +772,7 @@
         <v>6</v>
       </c>
       <c r="H5" s="2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>8</v>
@@ -744,16 +783,16 @@
     </row>
     <row r="6" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>30</v>
@@ -776,28 +815,28 @@
     </row>
     <row r="7" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H7" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>8</v>
@@ -808,46 +847,78 @@
     </row>
     <row r="8" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="H8" s="2">
+        <v>16</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{6A044975-EA9B-9C49-ADA3-1B2254AAB14F}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{6A30371D-97B6-0A4F-A002-26383FB13EC1}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{7758EFA3-9738-C74D-A092-6ABBEBB3BA66}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{8825CE27-BE97-F140-AE41-256163D1CC73}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{9C3858EA-0D79-3C40-A775-DD6592C6502A}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{40A9C183-943D-1B41-93AE-4D667EE568A5}"/>
-    <hyperlink ref="A7" r:id="rId7" xr:uid="{664AE765-5EDE-694E-A6C2-D63C76CCDA9B}"/>
-    <hyperlink ref="A8" r:id="rId8" xr:uid="{0F3FC39D-6E95-534E-BAF4-BAB7531DA6F8}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6A044975-EA9B-9C49-ADA3-1B2254AAB14F}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{6A30371D-97B6-0A4F-A002-26383FB13EC1}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{7758EFA3-9738-C74D-A092-6ABBEBB3BA66}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{8825CE27-BE97-F140-AE41-256163D1CC73}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{9C3858EA-0D79-3C40-A775-DD6592C6502A}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{40A9C183-943D-1B41-93AE-4D667EE568A5}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{664AE765-5EDE-694E-A6C2-D63C76CCDA9B}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{0F3FC39D-6E95-534E-BAF4-BAB7531DA6F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>